<commit_message>
Refactor testing data table reader
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/NominalPartitionTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/NominalPartitionTest.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25095" windowHeight="6330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25095" windowHeight="6330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test 10x5 radix" sheetId="1" r:id="rId1"/>
+    <sheet name="definitions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -364,8 +365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -629,4 +630,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>